<commit_message>
Change line 216 all.x=FALSE to remove year 2017 with NA value. Fixes error in for loop on line 264.
</commit_message>
<xml_diff>
--- a/data_out/check_update_process_data_for_loop_error.xlsx
+++ b/data_out/check_update_process_data_for_loop_error.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\nicola_chinook\data_out\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F181650A-6D45-43E1-BBCB-8EA6400E90A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46A359EC-7D59-4438-9B2E-DDED1C4111B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BC569C9A-57EA-48A7-A59C-1B769C5DF364}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BC569C9A-57EA-48A7-A59C-1B769C5DF364}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="15">
   <si>
     <t>return_age</t>
   </si>
@@ -73,6 +73,12 @@
   </si>
   <si>
     <t>hatchery_spawners</t>
+  </si>
+  <si>
+    <t>OLD (line 216: all.x=TRUE)</t>
+  </si>
+  <si>
+    <t>NEW  (line 216: all.x=TRUE)</t>
   </si>
 </sst>
 </file>
@@ -450,24 +456,27 @@
   <dimension ref="A1:X103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M78" sqref="M78"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
-    <col min="7" max="7" width="24.85546875" customWidth="1"/>
-    <col min="11" max="11" width="7.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" customWidth="1"/>
+    <col min="7" max="7" width="24.88671875" customWidth="1"/>
+    <col min="11" max="11" width="7.88671875" customWidth="1"/>
+    <col min="13" max="13" width="13.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -476,7 +485,7 @@
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="I2" s="2" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
@@ -486,7 +495,7 @@
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -530,7 +539,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -602,7 +611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -658,7 +667,7 @@
         <v>0</v>
       </c>
       <c r="U5">
-        <f t="shared" si="0"/>
+        <f>L5-D5</f>
         <v>-5</v>
       </c>
       <c r="V5">
@@ -666,15 +675,15 @@
         <v>0</v>
       </c>
       <c r="W5">
-        <f t="shared" si="0"/>
+        <f>N5-F5</f>
         <v>-5</v>
       </c>
       <c r="X5">
-        <f t="shared" si="0"/>
+        <f>O5-G5</f>
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>3</v>
       </c>
@@ -746,7 +755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>3</v>
       </c>
@@ -818,7 +827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>3</v>
       </c>
@@ -890,7 +899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>3</v>
       </c>
@@ -962,7 +971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>3</v>
       </c>
@@ -1034,7 +1043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>3</v>
       </c>
@@ -1106,7 +1115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>3</v>
       </c>
@@ -1178,7 +1187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>3</v>
       </c>
@@ -1250,7 +1259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>3</v>
       </c>
@@ -1322,7 +1331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>3</v>
       </c>
@@ -1394,7 +1403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>3</v>
       </c>
@@ -1466,7 +1475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>3</v>
       </c>
@@ -1538,7 +1547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>3</v>
       </c>
@@ -1610,7 +1619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>3</v>
       </c>
@@ -1682,7 +1691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>3</v>
       </c>
@@ -1754,7 +1763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>3</v>
       </c>
@@ -1826,7 +1835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>3</v>
       </c>
@@ -1898,7 +1907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>3</v>
       </c>
@@ -1970,7 +1979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>3</v>
       </c>
@@ -2042,7 +2051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>3</v>
       </c>
@@ -2114,7 +2123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>4</v>
       </c>
@@ -2186,7 +2195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>4</v>
       </c>
@@ -2258,7 +2267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>4</v>
       </c>
@@ -2314,7 +2323,7 @@
         <v>0</v>
       </c>
       <c r="U28">
-        <f t="shared" si="4"/>
+        <f>L28-D28</f>
         <v>-5</v>
       </c>
       <c r="V28">
@@ -2322,7 +2331,7 @@
         <v>0</v>
       </c>
       <c r="W28">
-        <f t="shared" si="6"/>
+        <f>N28-F28</f>
         <v>-4</v>
       </c>
       <c r="X28">
@@ -2330,7 +2339,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>4</v>
       </c>
@@ -2402,7 +2411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>4</v>
       </c>
@@ -2474,7 +2483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>4</v>
       </c>
@@ -2546,7 +2555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>4</v>
       </c>
@@ -2618,7 +2627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>4</v>
       </c>
@@ -2690,7 +2699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>4</v>
       </c>
@@ -2762,7 +2771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>4</v>
       </c>
@@ -2834,7 +2843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>4</v>
       </c>
@@ -2906,7 +2915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>4</v>
       </c>
@@ -2978,7 +2987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>4</v>
       </c>
@@ -3050,7 +3059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>4</v>
       </c>
@@ -3122,7 +3131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>4</v>
       </c>
@@ -3194,7 +3203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>4</v>
       </c>
@@ -3266,7 +3275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>4</v>
       </c>
@@ -3338,7 +3347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>4</v>
       </c>
@@ -3410,7 +3419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>4</v>
       </c>
@@ -3482,7 +3491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>4</v>
       </c>
@@ -3554,7 +3563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>4</v>
       </c>
@@ -3626,7 +3635,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>4</v>
       </c>
@@ -3698,7 +3707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>4</v>
       </c>
@@ -3770,7 +3779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>5</v>
       </c>
@@ -3842,7 +3851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>5</v>
       </c>
@@ -3914,7 +3923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>5</v>
       </c>
@@ -3986,7 +3995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>5</v>
       </c>
@@ -4058,7 +4067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>5</v>
       </c>
@@ -4130,7 +4139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>5</v>
       </c>
@@ -4202,7 +4211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>5</v>
       </c>
@@ -4274,7 +4283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>5</v>
       </c>
@@ -4346,7 +4355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>5</v>
       </c>
@@ -4418,7 +4427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>5</v>
       </c>
@@ -4490,7 +4499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>5</v>
       </c>
@@ -4562,7 +4571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>5</v>
       </c>
@@ -4634,7 +4643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>5</v>
       </c>
@@ -4706,7 +4715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>5</v>
       </c>
@@ -4778,7 +4787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>5</v>
       </c>
@@ -4850,7 +4859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>5</v>
       </c>
@@ -4922,7 +4931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>5</v>
       </c>
@@ -4994,7 +5003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>5</v>
       </c>
@@ -5066,7 +5075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>5</v>
       </c>
@@ -5138,7 +5147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>5</v>
       </c>
@@ -5210,7 +5219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>5</v>
       </c>
@@ -5282,7 +5291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>5</v>
       </c>
@@ -5354,7 +5363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>5</v>
       </c>
@@ -5426,7 +5435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>5</v>
       </c>
@@ -5498,12 +5507,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="78" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="s">
         <v>7</v>
       </c>
@@ -5524,7 +5533,7 @@
       <c r="O78" s="5"/>
       <c r="P78" s="5"/>
     </row>
-    <row r="79" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>1</v>
       </c>
@@ -5550,7 +5559,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="80" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>1995</v>
       </c>
@@ -5592,7 +5601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>1996</v>
       </c>
@@ -5634,7 +5643,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="82" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>1997</v>
       </c>
@@ -5676,7 +5685,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="83" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>1998</v>
       </c>
@@ -5718,7 +5727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>1999</v>
       </c>
@@ -5760,7 +5769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>2000</v>
       </c>
@@ -5802,7 +5811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>2001</v>
       </c>
@@ -5844,7 +5853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>2002</v>
       </c>
@@ -5886,7 +5895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>2003</v>
       </c>
@@ -5928,7 +5937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>2004</v>
       </c>
@@ -5970,7 +5979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>2005</v>
       </c>
@@ -6012,7 +6021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>2006</v>
       </c>
@@ -6054,7 +6063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>2007</v>
       </c>
@@ -6096,7 +6105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>2008</v>
       </c>
@@ -6138,7 +6147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>2009</v>
       </c>
@@ -6180,7 +6189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>2010</v>
       </c>
@@ -6222,7 +6231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>2011</v>
       </c>
@@ -6264,7 +6273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>2012</v>
       </c>
@@ -6306,7 +6315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>2013</v>
       </c>
@@ -6348,7 +6357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>2014</v>
       </c>
@@ -6390,7 +6399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>2015</v>
       </c>
@@ -6432,7 +6441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>2016</v>
       </c>
@@ -6474,7 +6483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>2017</v>
       </c>
@@ -6516,7 +6525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>2018</v>
       </c>

</xml_diff>

<commit_message>
Rerun fish data processing, update unmarked_hatchery_returns_by_year.csv
</commit_message>
<xml_diff>
--- a/data_out/check_update_process_data_for_loop_error.xlsx
+++ b/data_out/check_update_process_data_for_loop_error.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\nicola_chinook\data_out\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46A359EC-7D59-4438-9B2E-DDED1C4111B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E5C7720-9D75-44B6-BC4D-8C94ABC30E91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BC569C9A-57EA-48A7-A59C-1B769C5DF364}"/>
   </bookViews>
@@ -455,8 +455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F91FF38-C31B-4198-91D4-C02BFBD471A1}">
   <dimension ref="A1:X103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="A109" sqref="A109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>